<commit_message>
Updating for portable fixes
</commit_message>
<xml_diff>
--- a/spec/fixtures/snapshots/simple_example/spreadsheet/output.xlsx
+++ b/spec/fixtures/snapshots/simple_example/spreadsheet/output.xlsx
@@ -7,8 +7,9 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="manual_sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="auto_sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -470,6 +471,182 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>SIMPLE EXAMPLE</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Run By</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Jack Shepard</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Organization</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Oceanic 6</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>first</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>last</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>dob</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>funny</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>ignore</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Bozo</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Clown</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2000-01-04</t>
+        </is>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>me</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Frank</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Rizzo</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>1902-03-17</t>
+        </is>
+      </c>
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>me</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Joey</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Shmoey</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>1999-04-04</t>
+        </is>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>me</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Completed At</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>9/22/2004 04:15 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Brought to you by no one</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>